<commit_message>
finished xls files of motorFailure and Spark Analysis
</commit_message>
<xml_diff>
--- a/results_analysis/spark_xx_0x_holdx.xlsx
+++ b/results_analysis/spark_xx_0x_holdx.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\MLTool_matlab\results_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F36AB99-3E38-4FCE-9849-6EFBEE724CE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39403594-A6A7-46CE-86A0-6AF632839962}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="734" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="734" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="acc_mean" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="31">
   <si>
     <t>Sparsiciation Method</t>
   </si>
@@ -124,10 +124,10 @@
     <t>XX DataSet 0x - hold 0x - HP (best)</t>
   </si>
   <si>
-    <t>XX DataSet 0x - hold 0x - MCC</t>
+    <t>XX DataSet 0x - hold 0x - MCC (Multiclass)</t>
   </si>
   <si>
-    <t>XX DataSet 0x - hold 0x - F1-Score</t>
+    <t>XX DataSet 0x - hold 0x - F1-Score (Macro-Averaged)</t>
   </si>
 </sst>
 </file>
@@ -995,8 +995,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1665,36 +1665,694 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8065C56F-AEED-4D36-9CB5-AF6203A45422}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:K1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="60" t="s">
         <v>29</v>
       </c>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
+      <c r="H1" s="60"/>
+      <c r="I1" s="60"/>
+      <c r="J1" s="60"/>
+      <c r="K1" s="60"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+    </row>
+    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+    </row>
+    <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="K4" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="3">
+        <v>1</v>
+      </c>
+      <c r="C5" s="3">
+        <v>1</v>
+      </c>
+      <c r="D5" s="52"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="53"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="4"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="54"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="15"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="4"/>
+      <c r="B7" s="1">
+        <v>2</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1</v>
+      </c>
+      <c r="D7" s="54"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="15"/>
+    </row>
+    <row r="8" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="5"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="55"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="56"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="3">
+        <v>1</v>
+      </c>
+      <c r="C9" s="3">
+        <v>1</v>
+      </c>
+      <c r="D9" s="57"/>
+      <c r="E9" s="58"/>
+      <c r="F9" s="58"/>
+      <c r="G9" s="58"/>
+      <c r="H9" s="58"/>
+      <c r="I9" s="58"/>
+      <c r="J9" s="58"/>
+      <c r="K9" s="59"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="4"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="54"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="15"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="4"/>
+      <c r="B11" s="1">
+        <v>2</v>
+      </c>
+      <c r="C11" s="1">
+        <v>1</v>
+      </c>
+      <c r="D11" s="54"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="15"/>
+    </row>
+    <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="5"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="55"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="56"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="3">
+        <v>1</v>
+      </c>
+      <c r="C13" s="3">
+        <v>1</v>
+      </c>
+      <c r="D13" s="57"/>
+      <c r="E13" s="58"/>
+      <c r="F13" s="58"/>
+      <c r="G13" s="58"/>
+      <c r="H13" s="58"/>
+      <c r="I13" s="58"/>
+      <c r="J13" s="58"/>
+      <c r="K13" s="59"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="4"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="54"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="13"/>
+      <c r="K14" s="15"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="4"/>
+      <c r="B15" s="1">
+        <v>2</v>
+      </c>
+      <c r="C15" s="1">
+        <v>1</v>
+      </c>
+      <c r="D15" s="54"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="13"/>
+      <c r="K15" s="15"/>
+    </row>
+    <row r="16" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="5"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="55"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="56"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" s="1">
+        <v>1</v>
+      </c>
+      <c r="C17" s="1">
+        <v>1</v>
+      </c>
+      <c r="D17" s="57"/>
+      <c r="E17" s="58"/>
+      <c r="F17" s="58"/>
+      <c r="G17" s="58"/>
+      <c r="H17" s="58"/>
+      <c r="I17" s="58"/>
+      <c r="J17" s="58"/>
+      <c r="K17" s="59"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="4"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" s="54"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="13"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="13"/>
+      <c r="K18" s="15"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="4"/>
+      <c r="B19" s="1">
+        <v>2</v>
+      </c>
+      <c r="C19" s="1">
+        <v>1</v>
+      </c>
+      <c r="D19" s="54"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="13"/>
+      <c r="K19" s="15"/>
+    </row>
+    <row r="20" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="5"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20" s="55"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="14"/>
+      <c r="K20" s="56"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:K1"/>
+  </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBF1E589-1659-439B-B1DA-4F9E028A9755}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:K1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="60" t="s">
         <v>30</v>
       </c>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
+      <c r="H1" s="60"/>
+      <c r="I1" s="60"/>
+      <c r="J1" s="60"/>
+      <c r="K1" s="60"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+    </row>
+    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+    </row>
+    <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="K4" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="3">
+        <v>1</v>
+      </c>
+      <c r="C5" s="3">
+        <v>1</v>
+      </c>
+      <c r="D5" s="52"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="53"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="4"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="54"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="15"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="4"/>
+      <c r="B7" s="1">
+        <v>2</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1</v>
+      </c>
+      <c r="D7" s="54"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="15"/>
+    </row>
+    <row r="8" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="5"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="55"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="56"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="3">
+        <v>1</v>
+      </c>
+      <c r="C9" s="3">
+        <v>1</v>
+      </c>
+      <c r="D9" s="57"/>
+      <c r="E9" s="58"/>
+      <c r="F9" s="58"/>
+      <c r="G9" s="58"/>
+      <c r="H9" s="58"/>
+      <c r="I9" s="58"/>
+      <c r="J9" s="58"/>
+      <c r="K9" s="59"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="4"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="54"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="15"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="4"/>
+      <c r="B11" s="1">
+        <v>2</v>
+      </c>
+      <c r="C11" s="1">
+        <v>1</v>
+      </c>
+      <c r="D11" s="54"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="15"/>
+    </row>
+    <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="5"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="55"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="56"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="3">
+        <v>1</v>
+      </c>
+      <c r="C13" s="3">
+        <v>1</v>
+      </c>
+      <c r="D13" s="57"/>
+      <c r="E13" s="58"/>
+      <c r="F13" s="58"/>
+      <c r="G13" s="58"/>
+      <c r="H13" s="58"/>
+      <c r="I13" s="58"/>
+      <c r="J13" s="58"/>
+      <c r="K13" s="59"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="4"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="54"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="13"/>
+      <c r="K14" s="15"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="4"/>
+      <c r="B15" s="1">
+        <v>2</v>
+      </c>
+      <c r="C15" s="1">
+        <v>1</v>
+      </c>
+      <c r="D15" s="54"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="13"/>
+      <c r="K15" s="15"/>
+    </row>
+    <row r="16" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="5"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="55"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="56"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" s="1">
+        <v>1</v>
+      </c>
+      <c r="C17" s="1">
+        <v>1</v>
+      </c>
+      <c r="D17" s="57"/>
+      <c r="E17" s="58"/>
+      <c r="F17" s="58"/>
+      <c r="G17" s="58"/>
+      <c r="H17" s="58"/>
+      <c r="I17" s="58"/>
+      <c r="J17" s="58"/>
+      <c r="K17" s="59"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="4"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" s="54"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="13"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="13"/>
+      <c r="K18" s="15"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="4"/>
+      <c r="B19" s="1">
+        <v>2</v>
+      </c>
+      <c r="C19" s="1">
+        <v>1</v>
+      </c>
+      <c r="D19" s="54"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="13"/>
+      <c r="K19" s="15"/>
+    </row>
+    <row r="20" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="5"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20" s="55"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="14"/>
+      <c r="K20" s="56"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:K1"/>
+  </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
@@ -1704,7 +2362,7 @@
   <dimension ref="A1:K53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2218,7 +2876,7 @@
   <dimension ref="A1:K53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2890,7 +3548,7 @@
   <dimension ref="A1:K53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3404,7 +4062,7 @@
   <dimension ref="A1:K53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3918,7 +4576,7 @@
   <dimension ref="A1:K53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4432,7 +5090,7 @@
   <dimension ref="A1:K53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4946,7 +5604,7 @@
   <dimension ref="A1:P53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection sqref="A1:P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5077,90 +5735,38 @@
       <c r="C5" s="21">
         <v>1</v>
       </c>
-      <c r="D5" s="50">
-        <v>6.25E-2</v>
-      </c>
-      <c r="E5" s="37">
-        <v>0.5</v>
-      </c>
-      <c r="F5" s="38">
-        <v>1</v>
-      </c>
-      <c r="G5" s="38">
-        <v>1</v>
-      </c>
-      <c r="H5" s="38">
-        <v>3</v>
-      </c>
-      <c r="I5" s="38">
-        <v>128</v>
-      </c>
-      <c r="J5" s="38">
-        <v>2</v>
-      </c>
-      <c r="K5" s="38">
-        <v>3</v>
-      </c>
-      <c r="L5" s="38">
-        <v>4</v>
-      </c>
-      <c r="M5" s="33">
-        <v>3.125E-2</v>
-      </c>
-      <c r="N5" s="36">
-        <v>0.05</v>
-      </c>
-      <c r="O5" s="38">
-        <v>2</v>
-      </c>
-      <c r="P5" s="39">
-        <v>1</v>
-      </c>
+      <c r="D5" s="50"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="38"/>
+      <c r="H5" s="38"/>
+      <c r="I5" s="38"/>
+      <c r="J5" s="38"/>
+      <c r="K5" s="38"/>
+      <c r="L5" s="38"/>
+      <c r="M5" s="33"/>
+      <c r="N5" s="36"/>
+      <c r="O5" s="38"/>
+      <c r="P5" s="39"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="C6" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="41">
-        <v>4</v>
-      </c>
-      <c r="E6" s="32">
-        <v>3.90625E-3</v>
-      </c>
-      <c r="F6" s="29">
-        <v>2</v>
-      </c>
-      <c r="G6" s="30">
-        <v>0.25</v>
-      </c>
-      <c r="H6" s="29">
-        <v>3</v>
-      </c>
-      <c r="I6" s="30">
-        <v>0.25</v>
-      </c>
-      <c r="J6" s="31">
-        <v>6.25E-2</v>
-      </c>
-      <c r="K6" s="19">
-        <v>2.6</v>
-      </c>
-      <c r="L6" s="31">
-        <v>6.25E-2</v>
-      </c>
-      <c r="M6" s="32">
-        <v>3.90625E-3</v>
-      </c>
-      <c r="N6" s="13">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="O6" s="19">
-        <v>0.5</v>
-      </c>
-      <c r="P6" s="15">
-        <v>0.125</v>
-      </c>
+      <c r="D6" s="41"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="29"/>
+      <c r="I6" s="30"/>
+      <c r="J6" s="31"/>
+      <c r="K6" s="19"/>
+      <c r="L6" s="31"/>
+      <c r="M6" s="32"/>
+      <c r="N6" s="13"/>
+      <c r="O6" s="19"/>
+      <c r="P6" s="15"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
@@ -5170,45 +5776,19 @@
       <c r="C7" s="22">
         <v>1</v>
       </c>
-      <c r="D7" s="41">
-        <v>8</v>
-      </c>
-      <c r="E7" s="19">
-        <v>0.5</v>
-      </c>
-      <c r="F7" s="19">
-        <v>0.5</v>
-      </c>
-      <c r="G7" s="29">
-        <v>8</v>
-      </c>
-      <c r="H7" s="29">
-        <v>3</v>
-      </c>
-      <c r="I7" s="30">
-        <v>0.25</v>
-      </c>
-      <c r="J7" s="32">
-        <v>3.125E-2</v>
-      </c>
-      <c r="K7" s="19">
-        <v>0.4</v>
-      </c>
-      <c r="L7" s="29">
-        <v>16</v>
-      </c>
-      <c r="M7" s="32">
-        <v>3.90625E-3</v>
-      </c>
-      <c r="N7" s="13">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="O7" s="32">
-        <v>7.8125E-3</v>
-      </c>
-      <c r="P7" s="44">
-        <v>0.25</v>
-      </c>
+      <c r="D7" s="41"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="29"/>
+      <c r="H7" s="29"/>
+      <c r="I7" s="30"/>
+      <c r="J7" s="32"/>
+      <c r="K7" s="19"/>
+      <c r="L7" s="29"/>
+      <c r="M7" s="32"/>
+      <c r="N7" s="13"/>
+      <c r="O7" s="32"/>
+      <c r="P7" s="44"/>
     </row>
     <row r="8" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5"/>
@@ -5216,45 +5796,19 @@
       <c r="C8" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="41">
-        <v>2</v>
-      </c>
-      <c r="E8" s="32">
-        <v>1.953125E-3</v>
-      </c>
-      <c r="F8" s="29">
-        <v>2</v>
-      </c>
-      <c r="G8" s="29">
-        <v>4</v>
-      </c>
-      <c r="H8" s="29">
-        <v>2</v>
-      </c>
-      <c r="I8" s="13">
-        <v>0.125</v>
-      </c>
-      <c r="J8" s="32">
-        <v>3.125E-2</v>
-      </c>
-      <c r="K8" s="29">
-        <v>2</v>
-      </c>
-      <c r="L8" s="29">
-        <v>32</v>
-      </c>
-      <c r="M8" s="32">
-        <v>1.5625E-2</v>
-      </c>
-      <c r="N8" s="13">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="O8" s="19">
-        <v>0.5</v>
-      </c>
-      <c r="P8" s="44">
-        <v>0.25</v>
-      </c>
+      <c r="D8" s="41"/>
+      <c r="E8" s="32"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="29"/>
+      <c r="H8" s="29"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="32"/>
+      <c r="K8" s="29"/>
+      <c r="L8" s="29"/>
+      <c r="M8" s="32"/>
+      <c r="N8" s="13"/>
+      <c r="O8" s="19"/>
+      <c r="P8" s="44"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
@@ -5266,90 +5820,38 @@
       <c r="C9" s="21">
         <v>1</v>
       </c>
-      <c r="D9" s="40">
-        <v>6.25E-2</v>
-      </c>
-      <c r="E9" s="19">
-        <v>0.5</v>
-      </c>
-      <c r="F9" s="29">
-        <v>4</v>
-      </c>
-      <c r="G9" s="31">
-        <v>6.25E-2</v>
-      </c>
-      <c r="H9" s="29">
-        <v>1</v>
-      </c>
-      <c r="I9" s="29">
-        <v>8</v>
-      </c>
-      <c r="J9" s="32">
-        <v>3.125E-2</v>
-      </c>
-      <c r="K9" s="19">
-        <v>2.4</v>
-      </c>
-      <c r="L9" s="29">
-        <v>1024</v>
-      </c>
-      <c r="M9" s="32">
-        <v>7.8125E-3</v>
-      </c>
-      <c r="N9" s="13">
-        <v>1E-3</v>
-      </c>
-      <c r="O9" s="32">
-        <v>3.90625E-3</v>
-      </c>
-      <c r="P9" s="43">
-        <v>6.25E-2</v>
-      </c>
+      <c r="D9" s="40"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="29"/>
+      <c r="G9" s="31"/>
+      <c r="H9" s="29"/>
+      <c r="I9" s="29"/>
+      <c r="J9" s="32"/>
+      <c r="K9" s="19"/>
+      <c r="L9" s="29"/>
+      <c r="M9" s="32"/>
+      <c r="N9" s="13"/>
+      <c r="O9" s="32"/>
+      <c r="P9" s="43"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="C10" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="40">
-        <v>6.25E-2</v>
-      </c>
-      <c r="E10" s="31">
-        <v>6.25E-2</v>
-      </c>
-      <c r="F10" s="29">
-        <v>2</v>
-      </c>
-      <c r="G10" s="29">
-        <v>2</v>
-      </c>
-      <c r="H10" s="19">
-        <v>0.6</v>
-      </c>
-      <c r="I10" s="31">
-        <v>6.25E-2</v>
-      </c>
-      <c r="J10" s="32">
-        <v>3.90625E-3</v>
-      </c>
-      <c r="K10" s="19">
-        <v>2.8</v>
-      </c>
-      <c r="L10" s="29">
-        <v>1</v>
-      </c>
-      <c r="M10" s="32">
-        <v>3.125E-2</v>
-      </c>
-      <c r="N10" s="19">
-        <v>0.1</v>
-      </c>
-      <c r="O10" s="29">
-        <v>8</v>
-      </c>
-      <c r="P10" s="44">
-        <v>0.25</v>
-      </c>
+      <c r="D10" s="40"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="29"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="31"/>
+      <c r="J10" s="32"/>
+      <c r="K10" s="19"/>
+      <c r="L10" s="29"/>
+      <c r="M10" s="32"/>
+      <c r="N10" s="19"/>
+      <c r="O10" s="29"/>
+      <c r="P10" s="44"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
@@ -5359,45 +5861,19 @@
       <c r="C11" s="22">
         <v>1</v>
       </c>
-      <c r="D11" s="41">
-        <v>1</v>
-      </c>
-      <c r="E11" s="19">
-        <v>0.5</v>
-      </c>
-      <c r="F11" s="31">
-        <v>6.25E-2</v>
-      </c>
-      <c r="G11" s="13">
-        <v>0.125</v>
-      </c>
-      <c r="H11" s="19">
-        <v>0.6</v>
-      </c>
-      <c r="I11" s="29">
-        <v>32</v>
-      </c>
-      <c r="J11" s="29">
-        <v>2</v>
-      </c>
-      <c r="K11" s="19">
-        <v>2.6</v>
-      </c>
-      <c r="L11" s="29">
-        <v>256</v>
-      </c>
-      <c r="M11" s="31">
-        <v>6.25E-2</v>
-      </c>
-      <c r="N11" s="13">
-        <v>1E-3</v>
-      </c>
-      <c r="O11" s="32">
-        <v>3.90625E-3</v>
-      </c>
-      <c r="P11" s="34">
-        <v>3.125E-2</v>
-      </c>
+      <c r="D11" s="41"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="31"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="19"/>
+      <c r="I11" s="29"/>
+      <c r="J11" s="29"/>
+      <c r="K11" s="19"/>
+      <c r="L11" s="29"/>
+      <c r="M11" s="31"/>
+      <c r="N11" s="13"/>
+      <c r="O11" s="32"/>
+      <c r="P11" s="34"/>
     </row>
     <row r="12" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
@@ -5405,45 +5881,19 @@
       <c r="C12" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="41">
-        <v>4</v>
-      </c>
-      <c r="E12" s="31">
-        <v>6.25E-2</v>
-      </c>
-      <c r="F12" s="13">
-        <v>0.125</v>
-      </c>
-      <c r="G12" s="13">
-        <v>0.125</v>
-      </c>
-      <c r="H12" s="19">
-        <v>0.8</v>
-      </c>
-      <c r="I12" s="31">
-        <v>6.25E-2</v>
-      </c>
-      <c r="J12" s="32">
-        <v>3.90625E-3</v>
-      </c>
-      <c r="K12" s="29">
-        <v>1</v>
-      </c>
-      <c r="L12" s="29">
-        <v>256</v>
-      </c>
-      <c r="M12" s="32">
-        <v>3.90625E-3</v>
-      </c>
-      <c r="N12" s="13">
-        <v>0.01</v>
-      </c>
-      <c r="O12" s="31">
-        <v>6.25E-2</v>
-      </c>
-      <c r="P12" s="43">
-        <v>6.25E-2</v>
-      </c>
+      <c r="D12" s="41"/>
+      <c r="E12" s="31"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="19"/>
+      <c r="I12" s="31"/>
+      <c r="J12" s="32"/>
+      <c r="K12" s="29"/>
+      <c r="L12" s="29"/>
+      <c r="M12" s="32"/>
+      <c r="N12" s="13"/>
+      <c r="O12" s="31"/>
+      <c r="P12" s="43"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
@@ -5455,90 +5905,38 @@
       <c r="C13" s="21">
         <v>1</v>
       </c>
-      <c r="D13" s="41">
-        <v>2</v>
-      </c>
-      <c r="E13" s="29">
-        <v>1</v>
-      </c>
-      <c r="F13" s="31">
-        <v>6.25E-2</v>
-      </c>
-      <c r="G13" s="30">
-        <v>0.25</v>
-      </c>
-      <c r="H13" s="19">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="I13" s="29">
-        <v>4</v>
-      </c>
-      <c r="J13" s="32">
-        <v>9.765625E-4</v>
-      </c>
-      <c r="K13" s="19">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="L13" s="29">
-        <v>4</v>
-      </c>
-      <c r="M13" s="13">
-        <v>0.125</v>
-      </c>
-      <c r="N13" s="13">
-        <v>1E-3</v>
-      </c>
-      <c r="O13" s="32">
-        <v>3.125E-2</v>
-      </c>
-      <c r="P13" s="45">
-        <v>1</v>
-      </c>
+      <c r="D13" s="41"/>
+      <c r="E13" s="29"/>
+      <c r="F13" s="31"/>
+      <c r="G13" s="30"/>
+      <c r="H13" s="19"/>
+      <c r="I13" s="29"/>
+      <c r="J13" s="32"/>
+      <c r="K13" s="19"/>
+      <c r="L13" s="29"/>
+      <c r="M13" s="13"/>
+      <c r="N13" s="13"/>
+      <c r="O13" s="32"/>
+      <c r="P13" s="45"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="C14" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="41">
-        <v>8</v>
-      </c>
-      <c r="E14" s="32">
-        <v>1.5625E-2</v>
-      </c>
-      <c r="F14" s="29">
-        <v>4</v>
-      </c>
-      <c r="G14" s="13">
-        <v>0.125</v>
-      </c>
-      <c r="H14" s="29">
-        <v>2</v>
-      </c>
-      <c r="I14" s="32">
-        <v>1.953125E-3</v>
-      </c>
-      <c r="J14" s="32">
-        <v>3.90625E-3</v>
-      </c>
-      <c r="K14" s="19">
-        <v>2.6</v>
-      </c>
-      <c r="L14" s="32">
-        <v>1.5625E-2</v>
-      </c>
-      <c r="M14" s="31">
-        <v>6.25E-2</v>
-      </c>
-      <c r="N14" s="30">
-        <v>0.05</v>
-      </c>
-      <c r="O14" s="29">
-        <v>2</v>
-      </c>
-      <c r="P14" s="15">
-        <v>0.125</v>
-      </c>
+      <c r="D14" s="41"/>
+      <c r="E14" s="32"/>
+      <c r="F14" s="29"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="29"/>
+      <c r="I14" s="32"/>
+      <c r="J14" s="32"/>
+      <c r="K14" s="19"/>
+      <c r="L14" s="32"/>
+      <c r="M14" s="31"/>
+      <c r="N14" s="30"/>
+      <c r="O14" s="29"/>
+      <c r="P14" s="15"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
@@ -5548,45 +5946,19 @@
       <c r="C15" s="22">
         <v>1</v>
       </c>
-      <c r="D15" s="41">
-        <v>8</v>
-      </c>
-      <c r="E15" s="29">
-        <v>1</v>
-      </c>
-      <c r="F15" s="30">
-        <v>0.25</v>
-      </c>
-      <c r="G15" s="29">
-        <v>8</v>
-      </c>
-      <c r="H15" s="29">
-        <v>1</v>
-      </c>
-      <c r="I15" s="29">
-        <v>64</v>
-      </c>
-      <c r="J15" s="29">
-        <v>512</v>
-      </c>
-      <c r="K15" s="19">
-        <v>0.8</v>
-      </c>
-      <c r="L15" s="32">
-        <v>7.8125E-3</v>
-      </c>
-      <c r="M15" s="29">
-        <v>1</v>
-      </c>
-      <c r="N15" s="30">
-        <v>0.05</v>
-      </c>
-      <c r="O15" s="32">
-        <v>3.90625E-3</v>
-      </c>
-      <c r="P15" s="43">
-        <v>6.25E-2</v>
-      </c>
+      <c r="D15" s="41"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="30"/>
+      <c r="G15" s="29"/>
+      <c r="H15" s="29"/>
+      <c r="I15" s="29"/>
+      <c r="J15" s="29"/>
+      <c r="K15" s="19"/>
+      <c r="L15" s="32"/>
+      <c r="M15" s="29"/>
+      <c r="N15" s="30"/>
+      <c r="O15" s="32"/>
+      <c r="P15" s="43"/>
     </row>
     <row r="16" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5"/>
@@ -5594,45 +5966,19 @@
       <c r="C16" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="D16" s="40">
-        <v>6.25E-2</v>
-      </c>
-      <c r="E16" s="29">
-        <v>128</v>
-      </c>
-      <c r="F16" s="29">
-        <v>2</v>
-      </c>
-      <c r="G16" s="19">
-        <v>0.5</v>
-      </c>
-      <c r="H16" s="19">
-        <v>0.6</v>
-      </c>
-      <c r="I16" s="29">
-        <v>1</v>
-      </c>
-      <c r="J16" s="32">
-        <v>9.765625E-4</v>
-      </c>
-      <c r="K16" s="29">
-        <v>2</v>
-      </c>
-      <c r="L16" s="29">
-        <v>256</v>
-      </c>
-      <c r="M16" s="32">
-        <v>7.8125E-3</v>
-      </c>
-      <c r="N16" s="19">
-        <v>0.1</v>
-      </c>
-      <c r="O16" s="30">
-        <v>0.25</v>
-      </c>
-      <c r="P16" s="45">
-        <v>32</v>
-      </c>
+      <c r="D16" s="40"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="29"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="19"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="32"/>
+      <c r="K16" s="29"/>
+      <c r="L16" s="29"/>
+      <c r="M16" s="32"/>
+      <c r="N16" s="19"/>
+      <c r="O16" s="30"/>
+      <c r="P16" s="45"/>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
@@ -5644,90 +5990,38 @@
       <c r="C17" s="22">
         <v>1</v>
       </c>
-      <c r="D17" s="40">
-        <v>6.25E-2</v>
-      </c>
-      <c r="E17" s="29">
-        <v>4</v>
-      </c>
-      <c r="F17" s="13">
-        <v>0.125</v>
-      </c>
-      <c r="G17" s="29">
-        <v>4</v>
-      </c>
-      <c r="H17" s="19">
-        <v>2.4</v>
-      </c>
-      <c r="I17" s="29">
-        <v>32</v>
-      </c>
-      <c r="J17" s="19">
-        <v>0.5</v>
-      </c>
-      <c r="K17" s="29">
-        <v>1</v>
-      </c>
-      <c r="L17" s="29">
-        <v>512</v>
-      </c>
-      <c r="M17" s="32">
-        <v>3.90625E-3</v>
-      </c>
-      <c r="N17" s="19">
-        <v>0.1</v>
-      </c>
-      <c r="O17" s="29">
-        <v>1</v>
-      </c>
-      <c r="P17" s="45">
-        <v>64</v>
-      </c>
+      <c r="D17" s="40"/>
+      <c r="E17" s="29"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="29"/>
+      <c r="H17" s="19"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="19"/>
+      <c r="K17" s="29"/>
+      <c r="L17" s="29"/>
+      <c r="M17" s="32"/>
+      <c r="N17" s="19"/>
+      <c r="O17" s="29"/>
+      <c r="P17" s="45"/>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="C18" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="D18" s="40">
-        <v>6.25E-2</v>
-      </c>
-      <c r="E18" s="32">
-        <v>3.90625E-3</v>
-      </c>
-      <c r="F18" s="29">
-        <v>2</v>
-      </c>
-      <c r="G18" s="29">
-        <v>2</v>
-      </c>
-      <c r="H18" s="29">
-        <v>3</v>
-      </c>
-      <c r="I18" s="29">
-        <v>8</v>
-      </c>
-      <c r="J18" s="32">
-        <v>7.8125E-3</v>
-      </c>
-      <c r="K18" s="29">
-        <v>2</v>
-      </c>
-      <c r="L18" s="29">
-        <v>1024</v>
-      </c>
-      <c r="M18" s="32">
-        <v>3.90625E-3</v>
-      </c>
-      <c r="N18" s="19">
-        <v>0.1</v>
-      </c>
-      <c r="O18" s="29">
-        <v>4</v>
-      </c>
-      <c r="P18" s="15">
-        <v>0.125</v>
-      </c>
+      <c r="D18" s="40"/>
+      <c r="E18" s="32"/>
+      <c r="F18" s="29"/>
+      <c r="G18" s="29"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="32"/>
+      <c r="K18" s="29"/>
+      <c r="L18" s="29"/>
+      <c r="M18" s="32"/>
+      <c r="N18" s="19"/>
+      <c r="O18" s="29"/>
+      <c r="P18" s="15"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
@@ -5737,45 +6031,19 @@
       <c r="C19" s="22">
         <v>1</v>
       </c>
-      <c r="D19" s="40">
-        <v>6.25E-2</v>
-      </c>
-      <c r="E19" s="19">
-        <v>0.5</v>
-      </c>
-      <c r="F19" s="29">
-        <v>2</v>
-      </c>
-      <c r="G19" s="29">
-        <v>8</v>
-      </c>
-      <c r="H19" s="19">
-        <v>2.6</v>
-      </c>
-      <c r="I19" s="13">
-        <v>0.125</v>
-      </c>
-      <c r="J19" s="31">
-        <v>6.25E-2</v>
-      </c>
-      <c r="K19" s="19">
-        <v>0.4</v>
-      </c>
-      <c r="L19" s="29">
-        <v>256</v>
-      </c>
-      <c r="M19" s="32">
-        <v>3.125E-2</v>
-      </c>
-      <c r="N19" s="13">
-        <v>1E-3</v>
-      </c>
-      <c r="O19" s="29">
-        <v>1</v>
-      </c>
-      <c r="P19" s="44">
-        <v>0.25</v>
-      </c>
+      <c r="D19" s="40"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="29"/>
+      <c r="G19" s="29"/>
+      <c r="H19" s="19"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="31"/>
+      <c r="K19" s="19"/>
+      <c r="L19" s="29"/>
+      <c r="M19" s="32"/>
+      <c r="N19" s="13"/>
+      <c r="O19" s="29"/>
+      <c r="P19" s="44"/>
     </row>
     <row r="20" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="5"/>
@@ -5783,45 +6051,19 @@
       <c r="C20" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="D20" s="42">
-        <v>8</v>
-      </c>
-      <c r="E20" s="35">
-        <v>1.5625E-2</v>
-      </c>
-      <c r="F20" s="49">
-        <v>4</v>
-      </c>
-      <c r="G20" s="47">
-        <v>0.25</v>
-      </c>
-      <c r="H20" s="48">
-        <v>2.8</v>
-      </c>
-      <c r="I20" s="35">
-        <v>3.125E-2</v>
-      </c>
-      <c r="J20" s="35">
-        <v>3.125E-2</v>
-      </c>
-      <c r="K20" s="48">
-        <v>0.4</v>
-      </c>
-      <c r="L20" s="49">
-        <v>256</v>
-      </c>
-      <c r="M20" s="35">
-        <v>3.125E-2</v>
-      </c>
-      <c r="N20" s="14">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="O20" s="46">
-        <v>6.25E-2</v>
-      </c>
-      <c r="P20" s="51">
-        <v>6.25E-2</v>
-      </c>
+      <c r="D20" s="42"/>
+      <c r="E20" s="35"/>
+      <c r="F20" s="49"/>
+      <c r="G20" s="47"/>
+      <c r="H20" s="48"/>
+      <c r="I20" s="35"/>
+      <c r="J20" s="35"/>
+      <c r="K20" s="48"/>
+      <c r="L20" s="49"/>
+      <c r="M20" s="35"/>
+      <c r="N20" s="14"/>
+      <c r="O20" s="46"/>
+      <c r="P20" s="51"/>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B22" s="11"/>
@@ -6081,7 +6323,7 @@
   <dimension ref="A1:S53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection sqref="A1:R1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6224,108 +6466,44 @@
       <c r="C5" s="3">
         <v>1</v>
       </c>
-      <c r="D5" s="28">
-        <v>1.953125E-3</v>
-      </c>
-      <c r="E5" s="27">
-        <v>1024.001</v>
-      </c>
-      <c r="F5" s="28">
-        <v>1.5625E-2</v>
-      </c>
-      <c r="G5" s="27">
-        <v>1024.001</v>
-      </c>
-      <c r="H5" s="28">
-        <v>7.8125E-3</v>
-      </c>
-      <c r="I5" s="27">
-        <v>1024.001</v>
-      </c>
-      <c r="J5" s="12">
-        <v>1.953125E-3</v>
-      </c>
-      <c r="K5" s="27">
-        <v>1024.001</v>
-      </c>
-      <c r="L5" s="12">
-        <v>1.953125E-3</v>
-      </c>
-      <c r="M5" s="27">
-        <v>1024.001</v>
-      </c>
-      <c r="N5" s="12">
-        <v>-0.125</v>
-      </c>
-      <c r="O5" s="27">
-        <v>1024.001</v>
-      </c>
-      <c r="P5" s="28">
-        <v>1.953125E-3</v>
-      </c>
-      <c r="Q5" s="27">
-        <v>1024.001</v>
-      </c>
-      <c r="R5" s="28">
-        <v>1.953125E-3</v>
-      </c>
-      <c r="S5" s="27">
-        <v>1024.001</v>
-      </c>
+      <c r="D5" s="28"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="28"/>
+      <c r="G5" s="27"/>
+      <c r="H5" s="28"/>
+      <c r="I5" s="27"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="27"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="27"/>
+      <c r="N5" s="12"/>
+      <c r="O5" s="27"/>
+      <c r="P5" s="28"/>
+      <c r="Q5" s="27"/>
+      <c r="R5" s="28"/>
+      <c r="S5" s="27"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="C6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="31">
-        <v>3.90625E-3</v>
-      </c>
-      <c r="E6" s="29">
-        <v>1024.001</v>
-      </c>
-      <c r="F6" s="29">
-        <v>1</v>
-      </c>
-      <c r="G6" s="29">
-        <v>1024.001</v>
-      </c>
-      <c r="H6" s="30">
-        <v>0.25</v>
-      </c>
-      <c r="I6" s="29">
-        <v>1024.001</v>
-      </c>
-      <c r="J6" s="13">
-        <v>0.125</v>
-      </c>
-      <c r="K6" s="29">
-        <v>1024.001</v>
-      </c>
-      <c r="L6" s="30">
-        <v>0.25</v>
-      </c>
-      <c r="M6" s="29">
-        <v>1024.001</v>
-      </c>
-      <c r="N6" s="29">
-        <v>-8</v>
-      </c>
-      <c r="O6" s="29">
-        <v>1024.001</v>
-      </c>
-      <c r="P6" s="31">
-        <v>3.90625E-3</v>
-      </c>
-      <c r="Q6" s="29">
-        <v>1024.001</v>
-      </c>
-      <c r="R6" s="29">
-        <v>1</v>
-      </c>
-      <c r="S6" s="29">
-        <v>1024.001</v>
-      </c>
+      <c r="D6" s="31"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="29"/>
+      <c r="H6" s="30"/>
+      <c r="I6" s="29"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="29"/>
+      <c r="L6" s="30"/>
+      <c r="M6" s="29"/>
+      <c r="N6" s="29"/>
+      <c r="O6" s="29"/>
+      <c r="P6" s="31"/>
+      <c r="Q6" s="29"/>
+      <c r="R6" s="29"/>
+      <c r="S6" s="29"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
@@ -6335,54 +6513,22 @@
       <c r="C7" s="1">
         <v>1</v>
       </c>
-      <c r="D7" s="31">
-        <v>1.953125E-3</v>
-      </c>
-      <c r="E7" s="29">
-        <v>1024.001</v>
-      </c>
-      <c r="F7" s="31">
-        <v>6.25E-2</v>
-      </c>
-      <c r="G7" s="29">
-        <v>1024.001</v>
-      </c>
-      <c r="H7" s="31">
-        <v>7.8125E-3</v>
-      </c>
-      <c r="I7" s="29">
-        <v>1024.001</v>
-      </c>
-      <c r="J7" s="30">
-        <v>0.25</v>
-      </c>
-      <c r="K7" s="29">
-        <v>1024.001</v>
-      </c>
-      <c r="L7" s="29">
-        <v>1</v>
-      </c>
-      <c r="M7" s="29">
-        <v>1024.001</v>
-      </c>
-      <c r="N7" s="31">
-        <v>-1.5625E-2</v>
-      </c>
-      <c r="O7" s="29">
-        <v>1024.001</v>
-      </c>
-      <c r="P7" s="31">
-        <v>1.953125E-3</v>
-      </c>
-      <c r="Q7" s="29">
-        <v>1024.001</v>
-      </c>
-      <c r="R7" s="30">
-        <v>0.25</v>
-      </c>
-      <c r="S7" s="29">
-        <v>1024.001</v>
-      </c>
+      <c r="D7" s="31"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="29"/>
+      <c r="H7" s="31"/>
+      <c r="I7" s="29"/>
+      <c r="J7" s="30"/>
+      <c r="K7" s="29"/>
+      <c r="L7" s="29"/>
+      <c r="M7" s="29"/>
+      <c r="N7" s="31"/>
+      <c r="O7" s="29"/>
+      <c r="P7" s="31"/>
+      <c r="Q7" s="29"/>
+      <c r="R7" s="30"/>
+      <c r="S7" s="29"/>
     </row>
     <row r="8" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5"/>
@@ -6390,54 +6536,22 @@
       <c r="C8" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="31">
-        <v>3.90625E-3</v>
-      </c>
-      <c r="E8" s="29">
-        <v>1024.001</v>
-      </c>
-      <c r="F8" s="30">
-        <v>0.25</v>
-      </c>
-      <c r="G8" s="29">
-        <v>1024.001</v>
-      </c>
-      <c r="H8" s="29">
-        <v>64</v>
-      </c>
-      <c r="I8" s="29">
-        <v>1024.001</v>
-      </c>
-      <c r="J8" s="19">
-        <v>0.5</v>
-      </c>
-      <c r="K8" s="29">
-        <v>1024.001</v>
-      </c>
-      <c r="L8" s="19">
-        <v>0.5</v>
-      </c>
-      <c r="M8" s="29">
-        <v>1024.001</v>
-      </c>
-      <c r="N8" s="13">
-        <v>-0.125</v>
-      </c>
-      <c r="O8" s="29">
-        <v>1024.001</v>
-      </c>
-      <c r="P8" s="31">
-        <v>1.953125E-3</v>
-      </c>
-      <c r="Q8" s="29">
-        <v>1024.001</v>
-      </c>
-      <c r="R8" s="29">
-        <v>1</v>
-      </c>
-      <c r="S8" s="29">
-        <v>1024.001</v>
-      </c>
+      <c r="D8" s="31"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="29"/>
+      <c r="H8" s="29"/>
+      <c r="I8" s="29"/>
+      <c r="J8" s="19"/>
+      <c r="K8" s="29"/>
+      <c r="L8" s="19"/>
+      <c r="M8" s="29"/>
+      <c r="N8" s="13"/>
+      <c r="O8" s="29"/>
+      <c r="P8" s="31"/>
+      <c r="Q8" s="29"/>
+      <c r="R8" s="29"/>
+      <c r="S8" s="29"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
@@ -6449,108 +6563,44 @@
       <c r="C9" s="3">
         <v>1</v>
       </c>
-      <c r="D9" s="30">
-        <v>0.99</v>
-      </c>
-      <c r="E9" s="13">
-        <v>0.99099999999999999</v>
-      </c>
-      <c r="F9" s="19">
-        <v>0.5</v>
-      </c>
-      <c r="G9" s="13">
-        <v>0.99099999999999999</v>
-      </c>
-      <c r="H9" s="30">
-        <v>0.99</v>
-      </c>
-      <c r="I9" s="13">
-        <v>0.99099999999999999</v>
-      </c>
-      <c r="J9" s="30">
-        <v>0.99</v>
-      </c>
-      <c r="K9" s="13">
-        <v>0.99099999999999999</v>
-      </c>
-      <c r="L9" s="19">
-        <v>0.3</v>
-      </c>
-      <c r="M9" s="13">
-        <v>0.99099999999999999</v>
-      </c>
-      <c r="N9" s="19">
-        <v>0.4</v>
-      </c>
-      <c r="O9" s="29">
-        <v>1</v>
-      </c>
-      <c r="P9" s="30">
-        <v>0.99</v>
-      </c>
-      <c r="Q9" s="13">
-        <v>0.99099999999999999</v>
-      </c>
-      <c r="R9" s="19">
-        <v>0.1</v>
-      </c>
-      <c r="S9" s="13">
-        <v>0.99099999999999999</v>
-      </c>
+      <c r="D9" s="30"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="30"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="30"/>
+      <c r="K9" s="13"/>
+      <c r="L9" s="19"/>
+      <c r="M9" s="13"/>
+      <c r="N9" s="19"/>
+      <c r="O9" s="29"/>
+      <c r="P9" s="30"/>
+      <c r="Q9" s="13"/>
+      <c r="R9" s="19"/>
+      <c r="S9" s="13"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="C10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="30">
-        <v>0.99</v>
-      </c>
-      <c r="E10" s="13">
-        <v>0.99099999999999999</v>
-      </c>
-      <c r="F10" s="19">
-        <v>0.1</v>
-      </c>
-      <c r="G10" s="13">
-        <v>0.99099999999999999</v>
-      </c>
-      <c r="H10" s="30">
-        <v>0.99</v>
-      </c>
-      <c r="I10" s="13">
-        <v>0.99099999999999999</v>
-      </c>
-      <c r="J10" s="19">
-        <v>0.3</v>
-      </c>
-      <c r="K10" s="13">
-        <v>0.99099999999999999</v>
-      </c>
-      <c r="L10" s="30">
-        <v>0.01</v>
-      </c>
-      <c r="M10" s="13">
-        <v>0.99099999999999999</v>
-      </c>
-      <c r="N10" s="30">
-        <v>0.99</v>
-      </c>
-      <c r="O10" s="29">
-        <v>1</v>
-      </c>
-      <c r="P10" s="30">
-        <v>0.99</v>
-      </c>
-      <c r="Q10" s="13">
-        <v>0.99099999999999999</v>
-      </c>
-      <c r="R10" s="30">
-        <v>0.01</v>
-      </c>
-      <c r="S10" s="13">
-        <v>0.99099999999999999</v>
-      </c>
+      <c r="D10" s="30"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="30"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="19"/>
+      <c r="K10" s="13"/>
+      <c r="L10" s="30"/>
+      <c r="M10" s="13"/>
+      <c r="N10" s="30"/>
+      <c r="O10" s="29"/>
+      <c r="P10" s="30"/>
+      <c r="Q10" s="13"/>
+      <c r="R10" s="30"/>
+      <c r="S10" s="13"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
@@ -6560,54 +6610,22 @@
       <c r="C11" s="1">
         <v>1</v>
       </c>
-      <c r="D11" s="30">
-        <v>0.9</v>
-      </c>
-      <c r="E11" s="13">
-        <v>0.99099999999999999</v>
-      </c>
-      <c r="F11" s="30">
-        <v>0.9</v>
-      </c>
-      <c r="G11" s="13">
-        <v>0.99099999999999999</v>
-      </c>
-      <c r="H11" s="30">
-        <v>0.99</v>
-      </c>
-      <c r="I11" s="13">
-        <v>0.99099999999999999</v>
-      </c>
-      <c r="J11" s="30">
-        <v>0.99</v>
-      </c>
-      <c r="K11" s="13">
-        <v>0.99099999999999999</v>
-      </c>
-      <c r="L11" s="30">
-        <v>0.99</v>
-      </c>
-      <c r="M11" s="13">
-        <v>0.99099999999999999</v>
-      </c>
-      <c r="N11" s="19">
-        <v>0.7</v>
-      </c>
-      <c r="O11" s="29">
-        <v>1</v>
-      </c>
-      <c r="P11" s="30">
-        <v>0.99</v>
-      </c>
-      <c r="Q11" s="13">
-        <v>0.99099999999999999</v>
-      </c>
-      <c r="R11" s="19">
-        <v>0.1</v>
-      </c>
-      <c r="S11" s="13">
-        <v>0.99099999999999999</v>
-      </c>
+      <c r="D11" s="30"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="30"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="30"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="30"/>
+      <c r="K11" s="13"/>
+      <c r="L11" s="30"/>
+      <c r="M11" s="13"/>
+      <c r="N11" s="19"/>
+      <c r="O11" s="29"/>
+      <c r="P11" s="30"/>
+      <c r="Q11" s="13"/>
+      <c r="R11" s="19"/>
+      <c r="S11" s="13"/>
     </row>
     <row r="12" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
@@ -6615,54 +6633,22 @@
       <c r="C12" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="30">
-        <v>0.99</v>
-      </c>
-      <c r="E12" s="13">
-        <v>0.99099999999999999</v>
-      </c>
-      <c r="F12" s="30">
-        <v>0.01</v>
-      </c>
-      <c r="G12" s="13">
-        <v>0.99099999999999999</v>
-      </c>
-      <c r="H12" s="30">
-        <v>0.99</v>
-      </c>
-      <c r="I12" s="13">
-        <v>0.99099999999999999</v>
-      </c>
-      <c r="J12" s="19">
-        <v>0.1</v>
-      </c>
-      <c r="K12" s="13">
-        <v>0.99099999999999999</v>
-      </c>
-      <c r="L12" s="30">
-        <v>0.01</v>
-      </c>
-      <c r="M12" s="13">
-        <v>0.99099999999999999</v>
-      </c>
-      <c r="N12" s="19">
-        <v>0.8</v>
-      </c>
-      <c r="O12" s="29">
-        <v>1</v>
-      </c>
-      <c r="P12" s="30">
-        <v>0.99</v>
-      </c>
-      <c r="Q12" s="13">
-        <v>0.99099999999999999</v>
-      </c>
-      <c r="R12" s="19">
-        <v>0.1</v>
-      </c>
-      <c r="S12" s="13">
-        <v>0.99099999999999999</v>
-      </c>
+      <c r="D12" s="30"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="30"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="30"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="19"/>
+      <c r="K12" s="13"/>
+      <c r="L12" s="30"/>
+      <c r="M12" s="13"/>
+      <c r="N12" s="19"/>
+      <c r="O12" s="29"/>
+      <c r="P12" s="30"/>
+      <c r="Q12" s="13"/>
+      <c r="R12" s="19"/>
+      <c r="S12" s="13"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
@@ -6674,108 +6660,44 @@
       <c r="C13" s="3">
         <v>1</v>
       </c>
-      <c r="D13" s="31">
-        <v>3.90625E-3</v>
-      </c>
-      <c r="E13" s="29">
-        <v>4.0009765625</v>
-      </c>
-      <c r="F13" s="31">
-        <v>1.5625E-2</v>
-      </c>
-      <c r="G13" s="29">
-        <v>128.0009765625</v>
-      </c>
-      <c r="H13" s="31">
-        <v>1.953125E-3</v>
-      </c>
-      <c r="I13" s="13">
-        <v>0.5009765625</v>
-      </c>
-      <c r="J13" s="13">
-        <v>9.765625E-4</v>
-      </c>
-      <c r="K13" s="29">
-        <v>1024.0009765625</v>
-      </c>
-      <c r="L13" s="19">
-        <v>0.5</v>
-      </c>
-      <c r="M13" s="13">
-        <v>1.0009765625</v>
-      </c>
-      <c r="N13" s="31">
-        <v>1.953125E-3</v>
-      </c>
-      <c r="O13" s="31">
-        <v>8.7890625E-3</v>
-      </c>
-      <c r="P13" s="31">
-        <v>1.953125E-3</v>
-      </c>
-      <c r="Q13" s="31">
-        <v>1.66015625E-2</v>
-      </c>
-      <c r="R13" s="31">
-        <v>3.90625E-3</v>
-      </c>
-      <c r="S13" s="13">
-        <v>1.0009765625</v>
-      </c>
+      <c r="D13" s="31"/>
+      <c r="E13" s="29"/>
+      <c r="F13" s="31"/>
+      <c r="G13" s="29"/>
+      <c r="H13" s="31"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="13"/>
+      <c r="K13" s="29"/>
+      <c r="L13" s="19"/>
+      <c r="M13" s="13"/>
+      <c r="N13" s="31"/>
+      <c r="O13" s="31"/>
+      <c r="P13" s="31"/>
+      <c r="Q13" s="31"/>
+      <c r="R13" s="31"/>
+      <c r="S13" s="13"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="C14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="31">
-        <v>7.8125E-3</v>
-      </c>
-      <c r="E14" s="29">
-        <v>32.0009765625</v>
-      </c>
-      <c r="F14" s="31">
-        <v>7.8125E-3</v>
-      </c>
-      <c r="G14" s="31">
-        <v>8.7890625E-3</v>
-      </c>
-      <c r="H14" s="31">
-        <v>3.125E-2</v>
-      </c>
-      <c r="I14" s="29">
-        <v>512.0009765625</v>
-      </c>
-      <c r="J14" s="31">
-        <v>3.90625E-3</v>
-      </c>
-      <c r="K14" s="29">
-        <v>16.0009765625</v>
-      </c>
-      <c r="L14" s="13">
-        <v>0.125</v>
-      </c>
-      <c r="M14" s="29">
-        <v>512.0009765625</v>
-      </c>
-      <c r="N14" s="31">
-        <v>3.90625E-3</v>
-      </c>
-      <c r="O14" s="29">
-        <v>1.0009765625</v>
-      </c>
-      <c r="P14" s="31">
-        <v>9.765625E-4</v>
-      </c>
-      <c r="Q14" s="31">
-        <v>8.7890625E-3</v>
-      </c>
-      <c r="R14" s="31">
-        <v>1.5625E-2</v>
-      </c>
-      <c r="S14" s="13">
-        <v>1.0009765625</v>
-      </c>
+      <c r="D14" s="31"/>
+      <c r="E14" s="29"/>
+      <c r="F14" s="31"/>
+      <c r="G14" s="31"/>
+      <c r="H14" s="31"/>
+      <c r="I14" s="29"/>
+      <c r="J14" s="31"/>
+      <c r="K14" s="29"/>
+      <c r="L14" s="13"/>
+      <c r="M14" s="29"/>
+      <c r="N14" s="31"/>
+      <c r="O14" s="29"/>
+      <c r="P14" s="31"/>
+      <c r="Q14" s="31"/>
+      <c r="R14" s="31"/>
+      <c r="S14" s="13"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
@@ -6785,54 +6707,22 @@
       <c r="C15" s="1">
         <v>1</v>
       </c>
-      <c r="D15" s="29">
-        <v>2</v>
-      </c>
-      <c r="E15" s="13">
-        <v>0.1259765625</v>
-      </c>
-      <c r="F15" s="29">
-        <v>64</v>
-      </c>
-      <c r="G15" s="29">
-        <v>32.0009765625</v>
-      </c>
-      <c r="H15" s="29">
-        <v>256</v>
-      </c>
-      <c r="I15" s="19">
-        <v>0.5009765625</v>
-      </c>
-      <c r="J15" s="29">
-        <v>16</v>
-      </c>
-      <c r="K15" s="13">
-        <v>0.2509765625</v>
-      </c>
-      <c r="L15" s="29">
-        <v>8</v>
-      </c>
-      <c r="M15" s="29">
-        <v>64.0009765625</v>
-      </c>
-      <c r="N15" s="29">
-        <v>1</v>
-      </c>
-      <c r="O15" s="13">
-        <v>0.5009765625</v>
-      </c>
-      <c r="P15" s="29">
-        <v>16</v>
-      </c>
-      <c r="Q15" s="29">
-        <v>256.0009765625</v>
-      </c>
-      <c r="R15" s="29">
-        <v>512</v>
-      </c>
-      <c r="S15" s="13">
-        <v>2.0009765625</v>
-      </c>
+      <c r="D15" s="29"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="29"/>
+      <c r="G15" s="29"/>
+      <c r="H15" s="29"/>
+      <c r="I15" s="19"/>
+      <c r="J15" s="29"/>
+      <c r="K15" s="13"/>
+      <c r="L15" s="29"/>
+      <c r="M15" s="29"/>
+      <c r="N15" s="29"/>
+      <c r="O15" s="13"/>
+      <c r="P15" s="29"/>
+      <c r="Q15" s="29"/>
+      <c r="R15" s="29"/>
+      <c r="S15" s="13"/>
     </row>
     <row r="16" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5"/>
@@ -6840,54 +6730,22 @@
       <c r="C16" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D16" s="29">
-        <v>128</v>
-      </c>
-      <c r="E16" s="29">
-        <v>64.0009765625</v>
-      </c>
-      <c r="F16" s="29">
-        <v>1024</v>
-      </c>
-      <c r="G16" s="19">
-        <v>0.5009765625</v>
-      </c>
-      <c r="H16" s="13">
-        <v>9.765625E-4</v>
-      </c>
-      <c r="I16" s="29">
-        <v>2.0009765625</v>
-      </c>
-      <c r="J16" s="29">
-        <v>4</v>
-      </c>
-      <c r="K16" s="29">
-        <v>1.0009765625</v>
-      </c>
-      <c r="L16" s="31">
-        <v>3.90625E-3</v>
-      </c>
-      <c r="M16" s="29">
-        <v>64.0009765625</v>
-      </c>
-      <c r="N16" s="29">
-        <v>2</v>
-      </c>
-      <c r="O16" s="31">
-        <v>2.9296875E-3</v>
-      </c>
-      <c r="P16" s="13">
-        <v>9.765625E-4</v>
-      </c>
-      <c r="Q16" s="13">
-        <v>0.1259765625</v>
-      </c>
-      <c r="R16" s="29">
-        <v>32</v>
-      </c>
-      <c r="S16" s="13">
-        <v>0.2509765625</v>
-      </c>
+      <c r="D16" s="29"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="29"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="29"/>
+      <c r="K16" s="29"/>
+      <c r="L16" s="31"/>
+      <c r="M16" s="29"/>
+      <c r="N16" s="29"/>
+      <c r="O16" s="31"/>
+      <c r="P16" s="13"/>
+      <c r="Q16" s="13"/>
+      <c r="R16" s="29"/>
+      <c r="S16" s="13"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
@@ -6899,108 +6757,44 @@
       <c r="C17" s="1">
         <v>1</v>
       </c>
-      <c r="D17" s="29">
-        <v>16</v>
-      </c>
-      <c r="E17" s="29">
-        <v>1024.0009765625</v>
-      </c>
-      <c r="F17" s="29">
-        <v>16</v>
-      </c>
-      <c r="G17" s="29">
-        <v>256.0009765625</v>
-      </c>
-      <c r="H17" s="31">
-        <v>7.8125E-3</v>
-      </c>
-      <c r="I17" s="29">
-        <v>64.0009765625</v>
-      </c>
-      <c r="J17" s="31">
-        <v>1.5625E-2</v>
-      </c>
-      <c r="K17" s="31">
-        <v>6.34765625E-2</v>
-      </c>
-      <c r="L17" s="13">
-        <v>0.125</v>
-      </c>
-      <c r="M17" s="19">
-        <v>0.5009765625</v>
-      </c>
-      <c r="N17" s="29">
-        <v>-128</v>
-      </c>
-      <c r="O17" s="13">
-        <v>-9.765625E-4</v>
-      </c>
-      <c r="P17" s="31">
-        <v>3.90625E-3</v>
-      </c>
-      <c r="Q17" s="29">
-        <v>8.0009765625</v>
-      </c>
-      <c r="R17" s="29">
-        <v>8</v>
-      </c>
-      <c r="S17" s="29">
-        <v>128.0009765625</v>
-      </c>
+      <c r="D17" s="29"/>
+      <c r="E17" s="29"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="29"/>
+      <c r="H17" s="31"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="31"/>
+      <c r="K17" s="31"/>
+      <c r="L17" s="13"/>
+      <c r="M17" s="19"/>
+      <c r="N17" s="29"/>
+      <c r="O17" s="13"/>
+      <c r="P17" s="31"/>
+      <c r="Q17" s="29"/>
+      <c r="R17" s="29"/>
+      <c r="S17" s="29"/>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="C18" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D18" s="29">
-        <v>16</v>
-      </c>
-      <c r="E18" s="29">
-        <v>128.0009765625</v>
-      </c>
-      <c r="F18" s="31">
-        <v>1.5625E-2</v>
-      </c>
-      <c r="G18" s="19">
-        <v>0.5009765625</v>
-      </c>
-      <c r="H18" s="31">
-        <v>7.8125E-3</v>
-      </c>
-      <c r="I18" s="29">
-        <v>2.0009765625</v>
-      </c>
-      <c r="J18" s="29">
-        <v>1</v>
-      </c>
-      <c r="K18" s="29">
-        <v>256.0009765625</v>
-      </c>
-      <c r="L18" s="31">
-        <v>1.953125E-3</v>
-      </c>
-      <c r="M18" s="13">
-        <v>0.1259765625</v>
-      </c>
-      <c r="N18" s="31">
-        <v>-64</v>
-      </c>
-      <c r="O18" s="13">
-        <v>0.1259765625</v>
-      </c>
-      <c r="P18" s="13">
-        <v>9.765625E-4</v>
-      </c>
-      <c r="Q18" s="29">
-        <v>32.0009765625</v>
-      </c>
-      <c r="R18" s="31">
-        <v>1.953125E-3</v>
-      </c>
-      <c r="S18" s="29">
-        <v>16.0009765625</v>
-      </c>
+      <c r="D18" s="29"/>
+      <c r="E18" s="29"/>
+      <c r="F18" s="31"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="31"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="29"/>
+      <c r="K18" s="29"/>
+      <c r="L18" s="31"/>
+      <c r="M18" s="13"/>
+      <c r="N18" s="31"/>
+      <c r="O18" s="13"/>
+      <c r="P18" s="13"/>
+      <c r="Q18" s="29"/>
+      <c r="R18" s="31"/>
+      <c r="S18" s="29"/>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
@@ -7010,54 +6804,22 @@
       <c r="C19" s="1">
         <v>1</v>
       </c>
-      <c r="D19" s="31">
-        <v>6.25E-2</v>
-      </c>
-      <c r="E19" s="29">
-        <v>32.0009765625</v>
-      </c>
-      <c r="F19" s="30">
-        <v>0.25</v>
-      </c>
-      <c r="G19" s="29">
-        <v>64.0009765625</v>
-      </c>
-      <c r="H19" s="31">
-        <v>1.953125E-3</v>
-      </c>
-      <c r="I19" s="31">
-        <v>3.22265625E-2</v>
-      </c>
-      <c r="J19" s="31">
-        <v>3.125E-2</v>
-      </c>
-      <c r="K19" s="29">
-        <v>32.0009765625</v>
-      </c>
-      <c r="L19" s="31">
-        <v>1.5625E-2</v>
-      </c>
-      <c r="M19" s="29">
-        <v>16.0009765625</v>
-      </c>
-      <c r="N19" s="30">
-        <v>-0.25</v>
-      </c>
-      <c r="O19" s="29">
-        <v>32.0009765625</v>
-      </c>
-      <c r="P19" s="31">
-        <v>7.8125E-3</v>
-      </c>
-      <c r="Q19" s="29">
-        <v>8.0009765625</v>
-      </c>
-      <c r="R19" s="31">
-        <v>3.125E-2</v>
-      </c>
-      <c r="S19" s="13">
-        <v>0.5009765625</v>
-      </c>
+      <c r="D19" s="31"/>
+      <c r="E19" s="29"/>
+      <c r="F19" s="30"/>
+      <c r="G19" s="29"/>
+      <c r="H19" s="31"/>
+      <c r="I19" s="31"/>
+      <c r="J19" s="31"/>
+      <c r="K19" s="29"/>
+      <c r="L19" s="31"/>
+      <c r="M19" s="29"/>
+      <c r="N19" s="30"/>
+      <c r="O19" s="29"/>
+      <c r="P19" s="31"/>
+      <c r="Q19" s="29"/>
+      <c r="R19" s="31"/>
+      <c r="S19" s="13"/>
     </row>
     <row r="20" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="5"/>
@@ -7065,54 +6827,22 @@
       <c r="C20" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D20" s="31">
-        <v>1.5625E-2</v>
-      </c>
-      <c r="E20" s="29">
-        <v>32.0009765625</v>
-      </c>
-      <c r="F20" s="31">
-        <v>1.953125E-3</v>
-      </c>
-      <c r="G20" s="31">
-        <v>4.8828125E-3</v>
-      </c>
-      <c r="H20" s="31">
-        <v>7.8125E-3</v>
-      </c>
-      <c r="I20" s="13">
-        <v>0.5009765625</v>
-      </c>
-      <c r="J20" s="31">
-        <v>3.125E-2</v>
-      </c>
-      <c r="K20" s="31">
-        <v>6.34765625E-2</v>
-      </c>
-      <c r="L20" s="31">
-        <v>1.5625E-2</v>
-      </c>
-      <c r="M20" s="29">
-        <v>1.0009765625</v>
-      </c>
-      <c r="N20" s="29">
-        <v>4</v>
-      </c>
-      <c r="O20" s="29">
-        <v>8.0009765625</v>
-      </c>
-      <c r="P20" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="Q20" s="13">
-        <v>0.5009765625</v>
-      </c>
-      <c r="R20" s="31">
-        <v>1.953125E-3</v>
-      </c>
-      <c r="S20" s="13">
-        <v>0.5009765625</v>
-      </c>
+      <c r="D20" s="31"/>
+      <c r="E20" s="29"/>
+      <c r="F20" s="31"/>
+      <c r="G20" s="31"/>
+      <c r="H20" s="31"/>
+      <c r="I20" s="13"/>
+      <c r="J20" s="31"/>
+      <c r="K20" s="31"/>
+      <c r="L20" s="31"/>
+      <c r="M20" s="29"/>
+      <c r="N20" s="29"/>
+      <c r="O20" s="29"/>
+      <c r="P20" s="13"/>
+      <c r="Q20" s="13"/>
+      <c r="R20" s="31"/>
+      <c r="S20" s="13"/>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B22" s="11"/>

</xml_diff>